<commit_message>
Capítulo dos revisado hasta versículo 10
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="294" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="294" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="364">
   <si>
     <t>id</t>
   </si>
@@ -101,7 +101,7 @@
     <t>María</t>
   </si>
   <si>
-    <t>María; madre; </t>
+    <t>María; madre;</t>
   </si>
   <si>
     <t>per12</t>
@@ -152,7 +152,7 @@
     <t>Juan el Bautista</t>
   </si>
   <si>
-    <t>Juan; </t>
+    <t>Juan;</t>
   </si>
   <si>
     <t>per19</t>
@@ -680,6 +680,9 @@
     <t>Judea</t>
   </si>
   <si>
+    <t>Judá; tierra de Judá; </t>
+  </si>
+  <si>
     <t>pla3</t>
   </si>
   <si>
@@ -917,6 +920,15 @@
     <t>pla39</t>
   </si>
   <si>
+    <t>oriente</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Lugar del que proceden los magos que alaban a Jesús</t>
+  </si>
+  <si>
     <t>pla40</t>
   </si>
   <si>
@@ -1004,6 +1016,9 @@
     <t>org13</t>
   </si>
   <si>
+    <t>judíos</t>
+  </si>
+  <si>
     <t>org14</t>
   </si>
   <si>
@@ -1043,7 +1058,7 @@
     <t>tim2</t>
   </si>
   <si>
-    <t>Día del juicio; fin del mundo; </t>
+    <t>Día del juicio; fin del mundo;</t>
   </si>
   <si>
     <t>Tribulación de aquellos Días; fin</t>
@@ -1089,6 +1104,9 @@
   </si>
   <si>
     <t>tim8</t>
+  </si>
+  <si>
+    <t>días del Rey Herodes</t>
   </si>
   <si>
     <t>tim9</t>
@@ -1213,7 +1231,7 @@
   </sheetPr>
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
@@ -2113,10 +2131,10 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2152,326 +2170,338 @@
       <c r="B3" s="0" t="s">
         <v>219</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -2495,7 +2525,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2513,149 +2543,152 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2712,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2695,88 +2728,91 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>356</v>
+        <v>361</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hasta capítulo 7 revisado
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="294" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="144" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="366">
   <si>
     <t>id</t>
   </si>
@@ -680,7 +680,7 @@
     <t>Judea</t>
   </si>
   <si>
-    <t>Judá; tierra de Judá; </t>
+    <t>Judá; tierra de Judá;</t>
   </si>
   <si>
     <t>pla3</t>
@@ -689,7 +689,7 @@
     <t>Jerusalén</t>
   </si>
   <si>
-    <t>ciudad del Gran Rey</t>
+    <t>ciudad del Gran Rey; santa ciudad</t>
   </si>
   <si>
     <t>pla4</t>
@@ -731,7 +731,7 @@
     <t>pla10</t>
   </si>
   <si>
-    <t>santa ciudad</t>
+    <t>Antes este id tenía el valor de “ciudad santa”, ahora integrado en pla3</t>
   </si>
   <si>
     <t>pla11</t>
@@ -794,7 +794,7 @@
     <t>reino de los cielos</t>
   </si>
   <si>
-    <t>reino de Dios</t>
+    <t>reino de Dios; tu reino</t>
   </si>
   <si>
     <t>pla20</t>
@@ -932,7 +932,13 @@
     <t>pla40</t>
   </si>
   <si>
+    <t>Decápolis</t>
+  </si>
+  <si>
     <t>pla41</t>
+  </si>
+  <si>
+    <t>tierra</t>
   </si>
   <si>
     <t>org1</t>
@@ -1232,9 +1238,9 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2132,9 +2138,9 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2154,6 +2160,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -2233,11 +2242,11 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2498,10 +2507,16 @@
       <c r="A41" s="0" t="s">
         <v>303</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2543,152 +2558,152 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2728,91 +2743,91 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corregido hasta el capítulo 11
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="144" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="213" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="512">
   <si>
     <t>id</t>
   </si>
@@ -668,6 +668,336 @@
     <t>Urías</t>
   </si>
   <si>
+    <t>per97</t>
+  </si>
+  <si>
+    <t>suegra de Pedro</t>
+  </si>
+  <si>
+    <t>per98</t>
+  </si>
+  <si>
+    <t>per99</t>
+  </si>
+  <si>
+    <t>per100</t>
+  </si>
+  <si>
+    <t>per101</t>
+  </si>
+  <si>
+    <t>per102</t>
+  </si>
+  <si>
+    <t>per103</t>
+  </si>
+  <si>
+    <t>per104</t>
+  </si>
+  <si>
+    <t>per105</t>
+  </si>
+  <si>
+    <t>per106</t>
+  </si>
+  <si>
+    <t>per107</t>
+  </si>
+  <si>
+    <t>per108</t>
+  </si>
+  <si>
+    <t>per109</t>
+  </si>
+  <si>
+    <t>per110</t>
+  </si>
+  <si>
+    <t>per111</t>
+  </si>
+  <si>
+    <t>per112</t>
+  </si>
+  <si>
+    <t>per113</t>
+  </si>
+  <si>
+    <t>per114</t>
+  </si>
+  <si>
+    <t>per115</t>
+  </si>
+  <si>
+    <t>per116</t>
+  </si>
+  <si>
+    <t>per117</t>
+  </si>
+  <si>
+    <t>per118</t>
+  </si>
+  <si>
+    <t>per119</t>
+  </si>
+  <si>
+    <t>per120</t>
+  </si>
+  <si>
+    <t>per121</t>
+  </si>
+  <si>
+    <t>per122</t>
+  </si>
+  <si>
+    <t>per123</t>
+  </si>
+  <si>
+    <t>per124</t>
+  </si>
+  <si>
+    <t>per125</t>
+  </si>
+  <si>
+    <t>per126</t>
+  </si>
+  <si>
+    <t>per127</t>
+  </si>
+  <si>
+    <t>per128</t>
+  </si>
+  <si>
+    <t>per129</t>
+  </si>
+  <si>
+    <t>per130</t>
+  </si>
+  <si>
+    <t>per131</t>
+  </si>
+  <si>
+    <t>per132</t>
+  </si>
+  <si>
+    <t>per133</t>
+  </si>
+  <si>
+    <t>per134</t>
+  </si>
+  <si>
+    <t>per135</t>
+  </si>
+  <si>
+    <t>per136</t>
+  </si>
+  <si>
+    <t>per137</t>
+  </si>
+  <si>
+    <t>per138</t>
+  </si>
+  <si>
+    <t>per139</t>
+  </si>
+  <si>
+    <t>per140</t>
+  </si>
+  <si>
+    <t>per141</t>
+  </si>
+  <si>
+    <t>per142</t>
+  </si>
+  <si>
+    <t>per143</t>
+  </si>
+  <si>
+    <t>per144</t>
+  </si>
+  <si>
+    <t>per145</t>
+  </si>
+  <si>
+    <t>per146</t>
+  </si>
+  <si>
+    <t>per147</t>
+  </si>
+  <si>
+    <t>per148</t>
+  </si>
+  <si>
+    <t>per149</t>
+  </si>
+  <si>
+    <t>per150</t>
+  </si>
+  <si>
+    <t>per151</t>
+  </si>
+  <si>
+    <t>per152</t>
+  </si>
+  <si>
+    <t>per153</t>
+  </si>
+  <si>
+    <t>per154</t>
+  </si>
+  <si>
+    <t>per155</t>
+  </si>
+  <si>
+    <t>per156</t>
+  </si>
+  <si>
+    <t>per157</t>
+  </si>
+  <si>
+    <t>per158</t>
+  </si>
+  <si>
+    <t>per159</t>
+  </si>
+  <si>
+    <t>per160</t>
+  </si>
+  <si>
+    <t>per161</t>
+  </si>
+  <si>
+    <t>per162</t>
+  </si>
+  <si>
+    <t>per163</t>
+  </si>
+  <si>
+    <t>per164</t>
+  </si>
+  <si>
+    <t>per165</t>
+  </si>
+  <si>
+    <t>per166</t>
+  </si>
+  <si>
+    <t>per167</t>
+  </si>
+  <si>
+    <t>per168</t>
+  </si>
+  <si>
+    <t>per169</t>
+  </si>
+  <si>
+    <t>per170</t>
+  </si>
+  <si>
+    <t>per171</t>
+  </si>
+  <si>
+    <t>per172</t>
+  </si>
+  <si>
+    <t>per173</t>
+  </si>
+  <si>
+    <t>per174</t>
+  </si>
+  <si>
+    <t>per175</t>
+  </si>
+  <si>
+    <t>per176</t>
+  </si>
+  <si>
+    <t>per177</t>
+  </si>
+  <si>
+    <t>per178</t>
+  </si>
+  <si>
+    <t>per179</t>
+  </si>
+  <si>
+    <t>per180</t>
+  </si>
+  <si>
+    <t>per181</t>
+  </si>
+  <si>
+    <t>per182</t>
+  </si>
+  <si>
+    <t>per183</t>
+  </si>
+  <si>
+    <t>per184</t>
+  </si>
+  <si>
+    <t>per185</t>
+  </si>
+  <si>
+    <t>per186</t>
+  </si>
+  <si>
+    <t>per187</t>
+  </si>
+  <si>
+    <t>per188</t>
+  </si>
+  <si>
+    <t>per189</t>
+  </si>
+  <si>
+    <t>per190</t>
+  </si>
+  <si>
+    <t>per191</t>
+  </si>
+  <si>
+    <t>per192</t>
+  </si>
+  <si>
+    <t>per193</t>
+  </si>
+  <si>
+    <t>per194</t>
+  </si>
+  <si>
+    <t>per195</t>
+  </si>
+  <si>
+    <t>per196</t>
+  </si>
+  <si>
+    <t>per197</t>
+  </si>
+  <si>
+    <t>per198</t>
+  </si>
+  <si>
+    <t>per199</t>
+  </si>
+  <si>
+    <t>per200</t>
+  </si>
+  <si>
+    <t>per201</t>
+  </si>
+  <si>
+    <t>per202</t>
+  </si>
+  <si>
+    <t>per203</t>
+  </si>
+  <si>
+    <t>per204</t>
+  </si>
+  <si>
+    <t>per205</t>
+  </si>
+  <si>
     <t>pla1</t>
   </si>
   <si>
@@ -941,6 +1271,99 @@
     <t>tierra</t>
   </si>
   <si>
+    <t>pla42</t>
+  </si>
+  <si>
+    <t>occidente</t>
+  </si>
+  <si>
+    <t>pla43</t>
+  </si>
+  <si>
+    <t>mar de Galilea</t>
+  </si>
+  <si>
+    <t>pla44</t>
+  </si>
+  <si>
+    <t>pla45</t>
+  </si>
+  <si>
+    <t>pla46</t>
+  </si>
+  <si>
+    <t>pla47</t>
+  </si>
+  <si>
+    <t>pla48</t>
+  </si>
+  <si>
+    <t>pla49</t>
+  </si>
+  <si>
+    <t>pla50</t>
+  </si>
+  <si>
+    <t>pla51</t>
+  </si>
+  <si>
+    <t>pla52</t>
+  </si>
+  <si>
+    <t>pla53</t>
+  </si>
+  <si>
+    <t>pla54</t>
+  </si>
+  <si>
+    <t>pla55</t>
+  </si>
+  <si>
+    <t>pla56</t>
+  </si>
+  <si>
+    <t>pla57</t>
+  </si>
+  <si>
+    <t>pla58</t>
+  </si>
+  <si>
+    <t>pla59</t>
+  </si>
+  <si>
+    <t>pla60</t>
+  </si>
+  <si>
+    <t>pla61</t>
+  </si>
+  <si>
+    <t>pla62</t>
+  </si>
+  <si>
+    <t>pla63</t>
+  </si>
+  <si>
+    <t>pla64</t>
+  </si>
+  <si>
+    <t>pla65</t>
+  </si>
+  <si>
+    <t>pla66</t>
+  </si>
+  <si>
+    <t>pla67</t>
+  </si>
+  <si>
+    <t>pla68</t>
+  </si>
+  <si>
+    <t>pla69</t>
+  </si>
+  <si>
+    <t>pla70</t>
+  </si>
+  <si>
     <t>org1</t>
   </si>
   <si>
@@ -1028,13 +1451,28 @@
     <t>org14</t>
   </si>
   <si>
+    <t>falsos profetas</t>
+  </si>
+  <si>
     <t>org15</t>
   </si>
   <si>
+    <t>enfermos</t>
+  </si>
+  <si>
+    <t>Leprosos; paralíticos;</t>
+  </si>
+  <si>
     <t>org16</t>
   </si>
   <si>
+    <t>gentiles</t>
+  </si>
+  <si>
     <t>org17</t>
+  </si>
+  <si>
+    <t>samaritanos</t>
   </si>
   <si>
     <t>org18</t>
@@ -1205,7 +1643,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1215,6 +1653,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1235,12 +1677,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2095,7 +2537,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>210</v>
       </c>
@@ -2103,7 +2545,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>212</v>
       </c>
@@ -2111,12 +2553,560 @@
         <v>213</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>214</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2135,12 +3125,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2166,357 +3156,508 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>216</v>
+        <v>326</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>217</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>218</v>
+        <v>328</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>219</v>
+        <v>329</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>220</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>221</v>
+        <v>331</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>222</v>
+        <v>332</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>223</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>224</v>
+        <v>334</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>225</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>226</v>
+        <v>336</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>227</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>228</v>
+        <v>338</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>229</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>230</v>
+        <v>340</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>231</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>232</v>
+        <v>342</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>233</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>234</v>
+        <v>344</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>235</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>236</v>
+        <v>346</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>237</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>238</v>
+        <v>348</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>239</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>240</v>
+        <v>350</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>241</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>242</v>
+        <v>352</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>243</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>244</v>
+        <v>354</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>245</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>246</v>
+        <v>356</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>247</v>
+        <v>357</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>248</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>249</v>
+        <v>359</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>250</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>251</v>
+        <v>361</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>252</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>254</v>
+        <v>364</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>255</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>256</v>
+        <v>366</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>257</v>
+        <v>367</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>258</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>259</v>
+        <v>369</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>260</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>261</v>
+        <v>371</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>262</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>263</v>
+        <v>373</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>264</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>265</v>
+        <v>375</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>266</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>267</v>
+        <v>377</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>268</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>269</v>
+        <v>379</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>270</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>271</v>
+        <v>381</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>272</v>
+        <v>382</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>273</v>
+        <v>383</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>274</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>275</v>
+        <v>385</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>276</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>277</v>
+        <v>387</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>278</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>279</v>
+        <v>389</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>280</v>
+        <v>390</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>281</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>282</v>
+        <v>392</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>283</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>284</v>
+        <v>394</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>285</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>286</v>
+        <v>396</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>287</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>288</v>
+        <v>398</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>289</v>
+        <v>399</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>290</v>
+        <v>400</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>291</v>
+        <v>401</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>292</v>
+        <v>402</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>293</v>
+        <v>403</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>294</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>295</v>
+        <v>405</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>296</v>
+        <v>406</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>297</v>
+        <v>407</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>298</v>
+        <v>408</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>299</v>
+        <v>409</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>300</v>
+        <v>410</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>301</v>
+        <v>411</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>302</v>
+        <v>412</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>303</v>
+        <v>413</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>305</v>
+        <v>415</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>306</v>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -2540,7 +3681,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2558,152 +3699,167 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>307</v>
+        <v>448</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>308</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>309</v>
+        <v>450</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>310</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>311</v>
+        <v>452</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>312</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>313</v>
+        <v>454</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>314</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>315</v>
+        <v>456</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>316</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>317</v>
+        <v>458</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>318</v>
+        <v>459</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>319</v>
+        <v>460</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>320</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>321</v>
+        <v>462</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>322</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>323</v>
+        <v>464</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>324</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>325</v>
+        <v>466</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>326</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>327</v>
+        <v>468</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>328</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>330</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>331</v>
+        <v>472</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>332</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>333</v>
+        <v>474</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>334</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>476</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>336</v>
+        <v>478</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>481</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>338</v>
+        <v>483</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>339</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>340</v>
+        <v>486</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>341</v>
+        <v>487</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>342</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -2727,7 +3883,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2743,91 +3899,91 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>343</v>
+        <v>489</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>344</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>345</v>
+        <v>491</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>346</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>493</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>348</v>
+        <v>494</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>349</v>
+        <v>495</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>350</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>351</v>
+        <v>497</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>352</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>354</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>355</v>
+        <v>501</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>356</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>357</v>
+        <v>503</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>358</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>359</v>
+        <v>505</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>360</v>
+        <v>506</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>361</v>
+        <v>507</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>362</v>
+        <v>508</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>363</v>
+        <v>509</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>364</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>365</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido hasta el capítulo 13
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="213" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="218" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="518">
   <si>
     <t>id</t>
   </si>
@@ -104,6 +104,9 @@
     <t>María; madre;</t>
   </si>
   <si>
+    <t>María madre de Jesús</t>
+  </si>
+  <si>
     <t>per12</t>
   </si>
   <si>
@@ -1286,15 +1289,24 @@
     <t>pla44</t>
   </si>
   <si>
+    <t>Corazín</t>
+  </si>
+  <si>
     <t>pla45</t>
   </si>
   <si>
+    <t>Betsaida</t>
+  </si>
+  <si>
     <t>pla46</t>
   </si>
   <si>
     <t>pla47</t>
   </si>
   <si>
+    <t>sinagoga</t>
+  </si>
+  <si>
     <t>pla48</t>
   </si>
   <si>
@@ -1478,6 +1490,9 @@
     <t>org18</t>
   </si>
   <si>
+    <t>creyentes</t>
+  </si>
+  <si>
     <t>org19</t>
   </si>
   <si>
@@ -1554,6 +1569,9 @@
   </si>
   <si>
     <t>tim9</t>
+  </si>
+  <si>
+    <t>sábado</t>
   </si>
 </sst>
 </file>
@@ -1679,10 +1697,10 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1799,1314 +1817,1317 @@
       <c r="C12" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>26</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3128,9 +3149,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3156,508 +3177,520 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3678,10 +3711,10 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3699,167 +3732,170 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -3883,7 +3919,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3899,91 +3935,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>511</v>
+        <v>516</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hasta el capítulo 15 corregido
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="218" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="218" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="523">
   <si>
     <t>id</t>
   </si>
@@ -680,6 +680,9 @@
     <t>per98</t>
   </si>
   <si>
+    <t>hermano de Jesús</t>
+  </si>
+  <si>
     <t>per99</t>
   </si>
   <si>
@@ -692,6 +695,9 @@
     <t>per102</t>
   </si>
   <si>
+    <t>hermano de Herodes</t>
+  </si>
+  <si>
     <t>per103</t>
   </si>
   <si>
@@ -1274,6 +1280,9 @@
     <t>tierra</t>
   </si>
   <si>
+    <t>mundo</t>
+  </si>
+  <si>
     <t>pla42</t>
   </si>
   <si>
@@ -1394,6 +1403,9 @@
     <t>discípulos</t>
   </si>
   <si>
+    <t>discípulos de Jesús</t>
+  </si>
+  <si>
     <t>org4</t>
   </si>
   <si>
@@ -1494,6 +1506,9 @@
   </si>
   <si>
     <t>org19</t>
+  </si>
+  <si>
+    <t>no creyentes</t>
   </si>
   <si>
     <t>org20</t>
@@ -1697,10 +1712,10 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="B102" activeCellId="0" sqref="B99:D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2594,540 +2609,570 @@
       <c r="A99" s="0" t="s">
         <v>219</v>
       </c>
+      <c r="B99" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D100" s="0" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3149,9 +3194,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B58" activeCellId="1" sqref="B99:D102 B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3177,520 +3222,523 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -3709,12 +3757,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="1" sqref="B99:D102 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3732,170 +3780,176 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>465</v>
+        <v>468</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -3919,7 +3973,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="B99:D102 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3935,94 +3989,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisado hasta el capítullo 17
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="218" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="13" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="524">
   <si>
     <t>id</t>
   </si>
@@ -1272,6 +1272,9 @@
   </si>
   <si>
     <t>Decápolis</t>
+  </si>
+  <si>
+    <t>Padre de Simón Pedro</t>
   </si>
   <si>
     <t>pla41</t>
@@ -1713,9 +1716,9 @@
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B102" activeCellId="0" sqref="B99:D102"/>
+      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3194,9 +3197,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B58" activeCellId="1" sqref="B99:D102 B58"/>
+      <selection pane="bottomLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3566,53 +3569,56 @@
       <c r="B41" s="0" t="s">
         <v>417</v>
       </c>
+      <c r="D41" s="0" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>393</v>
@@ -3620,125 +3626,125 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -3762,7 +3768,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="1" sqref="B99:D102 B9"/>
+      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3780,176 +3786,176 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -3973,7 +3979,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="B99:D102 B3"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3989,94 +3995,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido hasta el capítulo 20
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="13" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="13" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="548">
   <si>
     <t>id</t>
   </si>
@@ -1517,7 +1517,79 @@
     <t>org20</t>
   </si>
   <si>
+    <t>publicanos</t>
+  </si>
+  <si>
     <t>org21</t>
+  </si>
+  <si>
+    <t>prostitutas</t>
+  </si>
+  <si>
+    <t>org22</t>
+  </si>
+  <si>
+    <t>tribus de Israel</t>
+  </si>
+  <si>
+    <t>org23</t>
+  </si>
+  <si>
+    <t>org24</t>
+  </si>
+  <si>
+    <t>org25</t>
+  </si>
+  <si>
+    <t>org26</t>
+  </si>
+  <si>
+    <t>org27</t>
+  </si>
+  <si>
+    <t>org28</t>
+  </si>
+  <si>
+    <t>org29</t>
+  </si>
+  <si>
+    <t>org30</t>
+  </si>
+  <si>
+    <t>org31</t>
+  </si>
+  <si>
+    <t>org32</t>
+  </si>
+  <si>
+    <t>org33</t>
+  </si>
+  <si>
+    <t>org34</t>
+  </si>
+  <si>
+    <t>org35</t>
+  </si>
+  <si>
+    <t>org36</t>
+  </si>
+  <si>
+    <t>org37</t>
+  </si>
+  <si>
+    <t>org38</t>
+  </si>
+  <si>
+    <t>org39</t>
+  </si>
+  <si>
+    <t>org40</t>
+  </si>
+  <si>
+    <t>org41</t>
+  </si>
+  <si>
+    <t>org42</t>
   </si>
   <si>
     <t>variantes</t>
@@ -1715,7 +1787,7 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
@@ -3197,7 +3269,7 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
@@ -3763,12 +3835,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3932,7 +4004,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>494</v>
       </c>
@@ -3940,7 +4012,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>496</v>
       </c>
@@ -3948,14 +4020,128 @@
         <v>497</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -3979,7 +4165,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3995,94 +4181,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>500</v>
+        <v>524</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>501</v>
+        <v>525</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>502</v>
+        <v>526</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>503</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>504</v>
+        <v>528</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>506</v>
+        <v>530</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>507</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>508</v>
+        <v>532</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>509</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>510</v>
+        <v>534</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>511</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>512</v>
+        <v>536</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>513</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>514</v>
+        <v>538</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>515</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>516</v>
+        <v>540</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>517</v>
+        <v>541</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>518</v>
+        <v>542</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>519</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>520</v>
+        <v>544</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>521</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>522</v>
+        <v>546</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>523</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido hasta el capítulo 25
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="13" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="549">
   <si>
     <t>id</t>
   </si>
@@ -1533,6 +1533,9 @@
   </si>
   <si>
     <t>org23</t>
+  </si>
+  <si>
+    <t>falsos cristos</t>
   </si>
   <si>
     <t>org24</t>
@@ -1788,9 +1791,9 @@
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2293,7 +2296,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>126</v>
       </c>
@@ -3269,9 +3272,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3691,9 +3694,6 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>430</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3837,10 +3837,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4048,100 +4046,103 @@
       <c r="A24" s="0" t="s">
         <v>504</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -4162,10 +4163,10 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4181,94 +4182,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido hasta el capítulo 27
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="549">
   <si>
     <t>id</t>
   </si>
@@ -185,6 +185,9 @@
     <t>Simón</t>
   </si>
   <si>
+    <t>hijo de Zebedeo</t>
+  </si>
+  <si>
     <t>per22</t>
   </si>
   <si>
@@ -195,9 +198,6 @@
   </si>
   <si>
     <t>Jacobo</t>
-  </si>
-  <si>
-    <t>hijo de Zebedeo</t>
   </si>
   <si>
     <t>per24</t>
@@ -1790,10 +1790,10 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2001,7 +2001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>52</v>
       </c>
@@ -2011,24 +2011,30 @@
       <c r="C22" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,7 +2101,7 @@
         <v>75</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>76</v>
@@ -2244,7 +2250,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>113</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>116</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>219</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>220</v>
@@ -3838,7 +3844,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4163,10 +4169,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Corregido por completogit add -Agit add -A
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="552">
   <si>
     <t>id</t>
   </si>
@@ -404,7 +404,7 @@
     <t>per54</t>
   </si>
   <si>
-    <t>hombre de Cirene</t>
+    <t>hombre de Cirene que lleva la cruz de Jesús</t>
   </si>
   <si>
     <t>per55</t>
@@ -1541,7 +1541,16 @@
     <t>org24</t>
   </si>
   <si>
+    <t>soldados</t>
+  </si>
+  <si>
     <t>org25</t>
+  </si>
+  <si>
+    <t>ancianos</t>
+  </si>
+  <si>
+    <t>ancianos del pueblo de Israel</t>
   </si>
   <si>
     <t>org26</t>
@@ -1790,10 +1799,8 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3278,9 +3285,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3843,8 +3850,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4060,95 +4067,104 @@
       <c r="A25" s="0" t="s">
         <v>506</v>
       </c>
+      <c r="B25" s="0" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -4169,8 +4185,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4186,94 +4202,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
said cambiado a q, con type
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -12,13 +12,15 @@
     <sheet name="Lugar" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Organizaciones" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Momento" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Topics" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Obras" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="555">
   <si>
     <t>id</t>
   </si>
@@ -1674,6 +1676,15 @@
   </si>
   <si>
     <t>sábado</t>
+  </si>
+  <si>
+    <t>top1</t>
+  </si>
+  <si>
+    <t>wor1</t>
+  </si>
+  <si>
+    <t>antiguo testamtento</t>
   </si>
 </sst>
 </file>
@@ -1799,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3851,7 +3862,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4186,7 +4197,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4301,4 +4312,99 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>552</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
@ana para señalar a quién se habla, colocado en total para las q no dichas por jesús ni escritas
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="556">
   <si>
     <t>id</t>
   </si>
@@ -1556,6 +1556,9 @@
   </si>
   <si>
     <t>org26</t>
+  </si>
+  <si>
+    <t>criados de Herodes</t>
   </si>
   <si>
     <t>org27</t>
@@ -3862,7 +3865,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4097,85 +4100,88 @@
       <c r="A27" s="0" t="s">
         <v>511</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -4213,94 +4219,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -4338,15 +4344,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -4384,18 +4390,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colocado @ana en q dichas por Jesús, per1; habría que revisarlo personalmente en navegador
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="557">
   <si>
     <t>id</t>
   </si>
@@ -1562,6 +1562,9 @@
   </si>
   <si>
     <t>org27</t>
+  </si>
+  <si>
+    <t>discípulos de Juan el bautista</t>
   </si>
   <si>
     <t>org28</t>
@@ -3864,8 +3867,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4108,80 +4111,86 @@
       <c r="A28" s="0" t="s">
         <v>513</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -4219,94 +4228,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -4344,15 +4353,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -4390,18 +4399,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primer capítulo de Juan corregido
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="559">
   <si>
     <t>id</t>
   </si>
@@ -403,6 +403,9 @@
     <t>per53</t>
   </si>
   <si>
+    <t>Natanael</t>
+  </si>
+  <si>
     <t>per54</t>
   </si>
   <si>
@@ -1313,6 +1316,9 @@
   </si>
   <si>
     <t>pla46</t>
+  </si>
+  <si>
+    <t>Betábara</t>
   </si>
   <si>
     <t>pla47</t>
@@ -1816,8 +1822,8 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2330,957 +2336,960 @@
       <c r="A54" s="0" t="s">
         <v>126</v>
       </c>
+      <c r="B54" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>54</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>26</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>54</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>83</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>70</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3302,9 +3311,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3330,523 +3339,526 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -3867,8 +3879,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3886,311 +3898,311 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -4212,7 +4224,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4228,94 +4240,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -4353,15 +4365,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -4399,18 +4411,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corregido hasta el capítulo 4
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="563">
   <si>
     <t>id</t>
   </si>
@@ -706,6 +706,9 @@
     <t>per103</t>
   </si>
   <si>
+    <t>Nicodemo</t>
+  </si>
+  <si>
     <t>per104</t>
   </si>
   <si>
@@ -1330,10 +1333,19 @@
     <t>pla48</t>
   </si>
   <si>
+    <t>Caná</t>
+  </si>
+  <si>
     <t>pla49</t>
   </si>
   <si>
+    <t>Enón</t>
+  </si>
+  <si>
     <t>pla50</t>
+  </si>
+  <si>
+    <t>Salim</t>
   </si>
   <si>
     <t>pla51</t>
@@ -1822,8 +1834,8 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2781,515 +2793,518 @@
       <c r="A104" s="0" t="s">
         <v>227</v>
       </c>
+      <c r="B104" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3313,7 +3328,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3339,526 +3354,535 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3880,7 +3904,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3898,311 +3922,311 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -4224,7 +4248,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4240,94 +4264,94 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -4365,15 +4389,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -4411,18 +4435,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido hasta el capítulo 5
</commit_message>
<xml_diff>
--- a/esquema mateoTEI.xlsx
+++ b/esquema mateoTEI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="577">
   <si>
     <t>id</t>
   </si>
@@ -1366,9 +1366,18 @@
     <t>pla53</t>
   </si>
   <si>
+    <t>Puerta de las Ovejas</t>
+  </si>
+  <si>
+    <t>En Jerusalén</t>
+  </si>
+  <si>
     <t>pla54</t>
   </si>
   <si>
+    <t>Betesda</t>
+  </si>
+  <si>
     <t>pla55</t>
   </si>
   <si>
@@ -1709,6 +1718,30 @@
   </si>
   <si>
     <t>sábado</t>
+  </si>
+  <si>
+    <t>tim10</t>
+  </si>
+  <si>
+    <t>bodas de Caná</t>
+  </si>
+  <si>
+    <t>tim11</t>
+  </si>
+  <si>
+    <t>tim12</t>
+  </si>
+  <si>
+    <t>tim13</t>
+  </si>
+  <si>
+    <t>tim14</t>
+  </si>
+  <si>
+    <t>tim15</t>
+  </si>
+  <si>
+    <t>tim16</t>
   </si>
   <si>
     <t>top1</t>
@@ -1843,7 +1876,7 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D106" activeCellId="0" sqref="D106"/>
     </sheetView>
   </sheetViews>
@@ -3343,7 +3376,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3820,90 +3853,99 @@
       <c r="A54" s="0" t="s">
         <v>447</v>
       </c>
+      <c r="B54" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -3925,7 +3967,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3943,311 +3985,311 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -4266,10 +4308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4285,94 +4327,132 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>562</v>
+        <v>565</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -4410,15 +4490,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>563</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -4456,18 +4536,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>